<commit_message>
refactored scrape to add 2017/2018 genres
</commit_message>
<xml_diff>
--- a/assets/data/top2019.xlsx
+++ b/assets/data/top2019.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q51"/>
+  <dimension ref="A1:R51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,6 +452,11 @@
           <t>year</t>
         </is>
       </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>genre</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -513,6 +518,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>['canadian pop', 'pop', 'post-teen pop', 'viral pop']</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -574,6 +584,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>['latin', 'reggaeton flow', 'trap latino']</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -635,6 +650,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>['dance pop', 'pop', 'post-teen pop']</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -696,6 +716,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>['pop', 'uk pop']</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -757,6 +782,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>['dfw rap', 'melodic rap', 'rap']</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -818,6 +848,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>['pop', 'uk pop']</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -879,6 +914,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>['melodic rap']</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -940,6 +980,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>['pop', 'uk pop']</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1001,6 +1046,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>['country rap', 'lgbtq+ hip hop', 'pop rap']</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1062,6 +1112,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>['electropop', 'pop']</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1123,6 +1178,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>['latin', 'reggaeton', 'trap latino']</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1184,6 +1244,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>['electronic trap']</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1245,6 +1310,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>['pop', 'uk pop']</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1306,6 +1376,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>['panamanian pop', 'reggaeton']</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1367,6 +1442,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>['canadian hip hop', 'canadian pop', 'hip hop', 'pop rap', 'rap', 'toronto rap']</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1428,6 +1508,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>['dance pop', 'pop', 'pop rap', 'r&amp;b', 'rap']</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1489,6 +1574,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>['latin', 'reggaeton']</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1550,6 +1640,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>['dfw rap', 'melodic rap', 'rap']</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1611,6 +1706,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>['pop rap']</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1672,6 +1772,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>['escape room', 'minnesota hip hop', 'pop', 'pop rap', 'trap queen']</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1733,6 +1838,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>['pop house']</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1794,6 +1904,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>['country rap', 'lgbtq+ hip hop', 'pop rap']</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1855,6 +1970,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>['latin', 'reggaeton', 'reggaeton flow', 'trap latino']</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1916,6 +2036,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>['latin', 'reggaeton', 'reggaeton flow']</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1977,6 +2102,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>['electropop', 'pop']</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2038,6 +2168,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>['canadian pop', 'pop', 'post-teen pop', 'viral pop']</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2099,6 +2234,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>['australian pop']</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2160,6 +2300,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>['canadian hip hop', 'pop']</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2221,6 +2366,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>['latin', 'latin hip hop', 'reggaeton', 'tropical']</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2282,6 +2432,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>['latin', 'reggaeton']</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2343,6 +2498,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>['electropop', 'pop', 'tropical house']</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2404,6 +2564,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>['dance pop', 'pop', 'post-teen pop']</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2465,6 +2630,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>['latin', 'reggaeton']</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2526,6 +2696,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>['atl hip hop', 'atl trap', 'gangster rap', 'melodic rap', 'pop rap', 'rap', 'trap']</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2587,6 +2762,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>['dance pop', 'pop', 'post-teen pop']</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2648,6 +2828,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>['big room', 'edm', 'pop', 'progressive house', 'tropical house']</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2709,6 +2894,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>['panamanian pop', 'reggaeton']</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2770,6 +2960,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>['pop', 'uk pop']</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2831,6 +3026,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>['boy band', 'dance pop', 'pop', 'pop rock', 'post-teen pop']</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2892,6 +3092,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>['pop']</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2953,6 +3158,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>['edm', 'pop', 'tropical house']</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -3014,6 +3224,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>['pop', 'post-teen pop']</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -3075,6 +3290,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>['dance pop', 'pop']</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -3136,6 +3356,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>['alternative r&amp;b', 'pop']</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -3197,6 +3422,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>['r&amp;b en espanol']</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -3258,6 +3488,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>['brostep', 'progressive electro house']</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -3319,6 +3554,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t>['latin', 'latin hip hop', 'reggaeton', 'tropical']</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -3380,6 +3620,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t>['brostep', 'progressive electro house']</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -3441,6 +3686,11 @@
           <t>2019</t>
         </is>
       </c>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>['electropop', 'pop', 'tropical house']</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -3500,6 +3750,11 @@
       <c r="Q51" t="inlineStr">
         <is>
           <t>2019</t>
+        </is>
+      </c>
+      <c r="R51" t="inlineStr">
+        <is>
+          <t>['pop', 'uk pop']</t>
         </is>
       </c>
     </row>

</xml_diff>